<commit_message>
fixed logging of r2, adapted predict loop
</commit_message>
<xml_diff>
--- a/src/results/model_metrics/00_summary.xlsx
+++ b/src/results/model_metrics/00_summary.xlsx
@@ -1,87 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\github\XBorderCap-ML\src\results\model_metrics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BAA7C3-B59A-47F5-9C3C-5EA973FC065D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>ModelType</t>
-  </si>
-  <si>
-    <t>Dataset</t>
-  </si>
-  <si>
-    <t>Learning Rate</t>
-  </si>
-  <si>
-    <t>Weight Decay</t>
-  </si>
-  <si>
-    <t>Train Split</t>
-  </si>
-  <si>
-    <t>Batch size</t>
-  </si>
-  <si>
-    <t>Epochs</t>
-  </si>
-  <si>
-    <t>Train loss</t>
-  </si>
-  <si>
-    <t>Val loss</t>
-  </si>
-  <si>
-    <t>R2-Score</t>
-  </si>
-  <si>
-    <t>MAE</t>
-  </si>
-  <si>
-    <t>BaseModel</t>
-  </si>
-  <si>
-    <t>BASELINE_MAXBEX</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -96,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -420,94 +420,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ModelType</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Learning Rate</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Weight Decay</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Train Split</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Batch size</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Train loss</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Val loss</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Train-R2-Score</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Val-R2-Score</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Train-MAE</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Val-MAE</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>1E-3</v>
-      </c>
-      <c r="D2">
-        <v>1E-3</v>
-      </c>
-      <c r="E2">
-        <v>0.8</v>
-      </c>
-      <c r="F2">
-        <v>512</v>
-      </c>
-      <c r="G2">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BaseModel</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BL_FBMC</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="F2" t="n">
+        <v>256</v>
+      </c>
+      <c r="G2" t="n">
         <v>100</v>
       </c>
-      <c r="H2">
-        <v>0.2</v>
-      </c>
-      <c r="I2">
-        <v>0.72</v>
-      </c>
-      <c r="J2">
-        <v>-1.17</v>
-      </c>
-      <c r="K2">
-        <v>1084.0400390625</v>
+      <c r="H2" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="I2" t="n">
+        <v>4.58</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="L2" t="n">
+        <v>564.1820068359375</v>
+      </c>
+      <c r="M2" t="n">
+        <v>871.85302734375</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BaseModel</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BL_FBMC_TIME</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="F3" t="n">
+        <v>256</v>
+      </c>
+      <c r="G3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="I3" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-0.34</v>
+      </c>
+      <c r="L3" t="n">
+        <v>562.4219970703125</v>
+      </c>
+      <c r="M3" t="n">
+        <v>903.3319702148438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added PCA / changed LSTM Model
</commit_message>
<xml_diff>
--- a/src/results/model_metrics/00_summary.xlsx
+++ b/src/results/model_metrics/00_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q63"/>
+  <dimension ref="A1:Q89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4135,15 +4135,11 @@
           <t>MSELoss</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>0.000300</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>0.001000</t>
-        </is>
+      <c r="D63" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.001</v>
       </c>
       <c r="F63" t="n">
         <v>0.9</v>
@@ -4180,6 +4176,1544 @@
       </c>
       <c r="Q63" t="n">
         <v>313.8999938964844</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>BL_FBMC_FULL</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>MSELoss</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H64" t="n">
+        <v>256</v>
+      </c>
+      <c r="I64" t="n">
+        <v>50</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="L64" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="M64" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="O64" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="P64" t="n">
+        <v>507.614990234375</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>876.7059936523438</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>BL_FBMC_FULL</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>HuberLoss</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H65" t="n">
+        <v>256</v>
+      </c>
+      <c r="I65" t="n">
+        <v>50</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0</v>
+      </c>
+      <c r="O65" t="n">
+        <v>-0.74</v>
+      </c>
+      <c r="P65" t="n">
+        <v>800.1090087890625</v>
+      </c>
+      <c r="Q65" t="n">
+        <v>933.77001953125</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>BaseModel</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>MSELoss</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H66" t="n">
+        <v>512</v>
+      </c>
+      <c r="I66" t="n">
+        <v>50</v>
+      </c>
+      <c r="J66" t="n">
+        <v>3847.09</v>
+      </c>
+      <c r="K66" t="n">
+        <v>3847.09</v>
+      </c>
+      <c r="L66" t="n">
+        <v>9525.709999999999</v>
+      </c>
+      <c r="M66" t="n">
+        <v>9525.709999999999</v>
+      </c>
+      <c r="N66" t="n">
+        <v>-3844.19</v>
+      </c>
+      <c r="O66" t="n">
+        <v>-16061.26</v>
+      </c>
+      <c r="P66" t="n">
+        <v>48614.7578125</v>
+      </c>
+      <c r="Q66" t="n">
+        <v>72373.3671875</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>BaseModel</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>MSELoss</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H67" t="n">
+        <v>512</v>
+      </c>
+      <c r="I67" t="n">
+        <v>100</v>
+      </c>
+      <c r="J67" t="n">
+        <v>156.68</v>
+      </c>
+      <c r="K67" t="n">
+        <v>156.68</v>
+      </c>
+      <c r="L67" t="n">
+        <v>931.05</v>
+      </c>
+      <c r="M67" t="n">
+        <v>931.05</v>
+      </c>
+      <c r="N67" t="n">
+        <v>-155.59</v>
+      </c>
+      <c r="O67" t="n">
+        <v>-1230.47</v>
+      </c>
+      <c r="P67" t="n">
+        <v>9747.150390625</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>23016.02734375</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>BaseModel</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>MSELoss</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H68" t="n">
+        <v>2048</v>
+      </c>
+      <c r="I68" t="n">
+        <v>250</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="L68" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="M68" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="O68" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="P68" t="n">
+        <v>591.89599609375</v>
+      </c>
+      <c r="Q68" t="n">
+        <v>945.2420043945312</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>BaseModel</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>L1Loss</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H69" t="n">
+        <v>2048</v>
+      </c>
+      <c r="I69" t="n">
+        <v>250</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="L69" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="M69" t="n">
+        <v>1</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O69" t="n">
+        <v>-0.77</v>
+      </c>
+      <c r="P69" t="n">
+        <v>585.447021484375</v>
+      </c>
+      <c r="Q69" t="n">
+        <v>955.52099609375</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>BaseModel</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>HuberLoss</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H70" t="n">
+        <v>2048</v>
+      </c>
+      <c r="I70" t="n">
+        <v>250</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="M70" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O70" t="n">
+        <v>-0.75</v>
+      </c>
+      <c r="P70" t="n">
+        <v>587.2490234375</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>951.0020141601562</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>MSELoss</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H71" t="n">
+        <v>512</v>
+      </c>
+      <c r="I71" t="n">
+        <v>100</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="L71" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="M71" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="N71" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="O71" t="n">
+        <v>-0.38</v>
+      </c>
+      <c r="P71" t="n">
+        <v>603.156982421875</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>901.1370239257812</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>MSELoss</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H72" t="n">
+        <v>512</v>
+      </c>
+      <c r="I72" t="n">
+        <v>100</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="L72" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="M72" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="N72" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="O72" t="n">
+        <v>-0.59</v>
+      </c>
+      <c r="P72" t="n">
+        <v>647.0289916992188</v>
+      </c>
+      <c r="Q72" t="n">
+        <v>896.5469970703125</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>MSELoss</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H73" t="n">
+        <v>512</v>
+      </c>
+      <c r="I73" t="n">
+        <v>100</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="L73" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="M73" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="N73" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O73" t="n">
+        <v>-0.24</v>
+      </c>
+      <c r="P73" t="n">
+        <v>648.2139892578125</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>744.458984375</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>MSELoss</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H74" t="n">
+        <v>512</v>
+      </c>
+      <c r="I74" t="n">
+        <v>100</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="L74" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="M74" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="N74" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="O74" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="P74" t="n">
+        <v>672.4299926757812</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>766.2020263671875</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H75" t="n">
+        <v>64</v>
+      </c>
+      <c r="I75" t="n">
+        <v>50</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="M75" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="N75" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="O75" t="n">
+        <v>-0.44</v>
+      </c>
+      <c r="P75" t="n">
+        <v>810.02197265625</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>874.7849731445312</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>MSELoss</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H76" t="n">
+        <v>64</v>
+      </c>
+      <c r="I76" t="n">
+        <v>50</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="L76" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="M76" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="O76" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="P76" t="n">
+        <v>545.5029907226562</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>801.0709838867188</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H77" t="n">
+        <v>64</v>
+      </c>
+      <c r="I77" t="n">
+        <v>50</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="L77" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="N77" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O77" t="n">
+        <v>-0.16</v>
+      </c>
+      <c r="P77" t="n">
+        <v>606.0850219726562</v>
+      </c>
+      <c r="Q77" t="n">
+        <v>786.083984375</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H78" t="n">
+        <v>64</v>
+      </c>
+      <c r="I78" t="n">
+        <v>50</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="L78" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M78" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="N78" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O78" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="P78" t="n">
+        <v>631.3740234375</v>
+      </c>
+      <c r="Q78" t="n">
+        <v>776.9719848632812</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H79" t="n">
+        <v>64</v>
+      </c>
+      <c r="I79" t="n">
+        <v>50</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="L79" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M79" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="N79" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O79" t="n">
+        <v>-0.15</v>
+      </c>
+      <c r="P79" t="n">
+        <v>626.635009765625</v>
+      </c>
+      <c r="Q79" t="n">
+        <v>775.2570190429688</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>BL_FBMC_FULL</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H80" t="n">
+        <v>64</v>
+      </c>
+      <c r="I80" t="n">
+        <v>50</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="L80" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="M80" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="N80" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="O80" t="n">
+        <v>-0.22</v>
+      </c>
+      <c r="P80" t="n">
+        <v>631.3070068359375</v>
+      </c>
+      <c r="Q80" t="n">
+        <v>775.31298828125</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H81" t="n">
+        <v>64</v>
+      </c>
+      <c r="I81" t="n">
+        <v>50</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="L81" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M81" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="N81" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O81" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="P81" t="n">
+        <v>631.3740234375</v>
+      </c>
+      <c r="Q81" t="n">
+        <v>776.9719848632812</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>BL_FBMC_FULL</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H82" t="n">
+        <v>64</v>
+      </c>
+      <c r="I82" t="n">
+        <v>50</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="L82" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="M82" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="N82" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="O82" t="n">
+        <v>-0.22</v>
+      </c>
+      <c r="P82" t="n">
+        <v>631.3070068359375</v>
+      </c>
+      <c r="Q82" t="n">
+        <v>775.31298828125</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>BL_FBMC_FULL</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H83" t="n">
+        <v>64</v>
+      </c>
+      <c r="I83" t="n">
+        <v>50</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L83" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="M83" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="N83" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O83" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="P83" t="n">
+        <v>665.0880126953125</v>
+      </c>
+      <c r="Q83" t="n">
+        <v>797.197998046875</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H84" t="n">
+        <v>64</v>
+      </c>
+      <c r="I84" t="n">
+        <v>50</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="L84" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="M84" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="N84" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="O84" t="n">
+        <v>-0.64</v>
+      </c>
+      <c r="P84" t="n">
+        <v>736.5150146484375</v>
+      </c>
+      <c r="Q84" t="n">
+        <v>876.177001953125</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>BL_FBMC_FULL</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H85" t="n">
+        <v>64</v>
+      </c>
+      <c r="I85" t="n">
+        <v>50</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L85" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="M85" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="N85" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O85" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="P85" t="n">
+        <v>665.0880126953125</v>
+      </c>
+      <c r="Q85" t="n">
+        <v>797.197998046875</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>BL_FBMC_FULL</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G86" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H86" t="n">
+        <v>64</v>
+      </c>
+      <c r="I86" t="n">
+        <v>50</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="K86" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="L86" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="M86" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="N86" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="O86" t="n">
+        <v>-0.22</v>
+      </c>
+      <c r="P86" t="n">
+        <v>631.3070068359375</v>
+      </c>
+      <c r="Q86" t="n">
+        <v>775.31298828125</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>BL_FBMC_FULL</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G87" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H87" t="n">
+        <v>64</v>
+      </c>
+      <c r="I87" t="n">
+        <v>50</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L87" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="M87" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="N87" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O87" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="P87" t="n">
+        <v>665.0880126953125</v>
+      </c>
+      <c r="Q87" t="n">
+        <v>797.197998046875</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>AGG_FBMC</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>SmoothL1Loss</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H88" t="n">
+        <v>64</v>
+      </c>
+      <c r="I88" t="n">
+        <v>50</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="K88" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="L88" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="M88" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="N88" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O88" t="n">
+        <v>-0.17</v>
+      </c>
+      <c r="P88" t="n">
+        <v>629.4030151367188</v>
+      </c>
+      <c r="Q88" t="n">
+        <v>788.552001953125</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Net</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>BL_FBMC_FULL</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>MSELoss</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0.000300</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>0.003000</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H89" t="n">
+        <v>64</v>
+      </c>
+      <c r="I89" t="n">
+        <v>50</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="K89" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="L89" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="M89" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="N89" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="O89" t="n">
+        <v>-0.85</v>
+      </c>
+      <c r="P89" t="n">
+        <v>759.2529907226562</v>
+      </c>
+      <c r="Q89" t="n">
+        <v>897.77001953125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>